<commit_message>
Individuals sheet update for the Protein Ontogenies column
</commit_message>
<xml_diff>
--- a/tests/testthat/data/Parameters/Individuals.xlsx
+++ b/tests/testthat/data/Parameters/Individuals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnastasiiaKostiv\OneDrive - esqlabs GmbH\Documents\GitHub\shinyScenarioEditor\tests\testthat\data\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296CF23F-FCAD-4B65-9237-9701AEE5FCA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FECD1B-C6E9-4876-B2B5-36E08FEFF4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="300" windowWidth="21564" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Human</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>Container Path</t>
-  </si>
-  <si>
-    <t>Protein Ontogenies</t>
   </si>
 </sst>
 </file>
@@ -495,10 +492,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3892D2-FAF9-44EE-B239-FAC53541F5B5}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,7 +506,7 @@
     <col min="6" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -521,9 +518,6 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -715,15 +709,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="425f6c96-429f-484f-969b-f607df711986">
@@ -732,6 +717,15 @@
     <TaxCatchAll xmlns="dffc3f26-5269-4005-8a8e-580fd4bf242e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -754,14 +748,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78CA0B51-7456-4883-901E-100C95177B36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028903B1-0B22-4BE6-8A73-043144867A27}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -772,4 +758,12 @@
     <ds:schemaRef ds:uri="dffc3f26-5269-4005-8a8e-580fd4bf242e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78CA0B51-7456-4883-901E-100C95177B36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>